<commit_message>
commiting service lines to Branch X
</commit_message>
<xml_diff>
--- a/eclipse-workspace/CAS_Project/reports/Book1.xlsx
+++ b/eclipse-workspace/CAS_Project/reports/Book1.xlsx
@@ -1,23 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\eclipse-workspace\CAS_Project\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2304093\git\CAS_project\eclipse-workspace\CAS_Project\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D8E00FD-C297-4F8D-9669-F211D84B61B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D06701-FE68-4015-8B81-FF1AE7C035C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{7F006C87-247A-4BBB-A999-87762A7712EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="9" activeTab="17" xr2:uid="{7F006C87-247A-4BBB-A999-87762A7712EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" r:id="rId5" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId6" sheetId="3"/>
-    <sheet name="Sheet4" r:id="rId7" sheetId="4"/>
-    <sheet name="Sheet5" r:id="rId8" sheetId="5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet20" r:id="rId23" sheetId="20"/>
+    <sheet name="Sheet21" r:id="rId24" sheetId="21"/>
+    <sheet name="Sheet22" r:id="rId25" sheetId="22"/>
+    <sheet name="Sheet23" r:id="rId26" sheetId="23"/>
+    <sheet name="Sheet24" r:id="rId27" sheetId="24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
   <si>
     <t>About Cognizant</t>
   </si>
@@ -56,6 +75,59 @@
   </si>
   <si>
     <t>Ravi Kumar S: A Journey of Growth</t>
+  </si>
+  <si>
+    <t>Service Lines Home</t>
+  </si>
+  <si>
+    <t>Core Technologies &amp; Insights (CT&amp;I)</t>
+  </si>
+  <si>
+    <t>Enterprise Platform Services (EPS)</t>
+  </si>
+  <si>
+    <t>Industry Solutions Group (ISG)</t>
+  </si>
+  <si>
+    <t>Intuitive Operations &amp; Automation (IOA)</t>
+  </si>
+  <si>
+    <t>Software &amp; Platform Engineering (SPE)</t>
+  </si>
+  <si>
+    <t>Enablement: Application Lifecycle Management</t>
+  </si>
+  <si>
+    <t>Enablement: Project &amp; Program Management</t>
+  </si>
+  <si>
+    <t>Enablement: Delivery Excellence</t>
+  </si>
+  <si>
+    <t>Enablement: Global Solution Architecture (GSA)</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence &amp; Analytics (AI&amp;A)</t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT)</t>
+  </si>
+  <si>
+    <t>Cloud, Infrastructure &amp; Security (CIS)</t>
+  </si>
+  <si>
+    <t>Sustainability Services</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Core Technologies &amp; Insights (CT&amp;I)
+</t>
+  </si>
+  <si>
+    <t>Software &amp; Platform Engineering (SPE)
+</t>
   </si>
 </sst>
 </file>
@@ -410,104 +482,914 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C3CE9C-0573-4B79-9B83-9A145AE0F01F}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A6712A-0724-403A-9318-B5DFDEBE8665}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>